<commit_message>
expanded years analyzed for VA project
</commit_message>
<xml_diff>
--- a/projects/virginia/capacity_sweep/scenarios.xlsx
+++ b/projects/virginia/capacity_sweep/scenarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8116D27-3083-41BF-AFF0-4F44C91F3D4E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A7A4A8-DB5D-4321-958B-F3A255020FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1495,7 +1495,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="D3:F3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,8 +1585,8 @@
         <v>26</v>
       </c>
       <c r="C4" s="4">
-        <f>8631360/150</f>
-        <v>57542.400000000001</v>
+        <f>(8631360+25408156)/150</f>
+        <v>226930.10666666666</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1632,7 +1632,8 @@
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <v>1064984</v>
+        <f>1064984*1.05</f>
+        <v>1118233.2</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1842,7 +1843,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:F3"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1932,8 +1933,8 @@
         <v>26</v>
       </c>
       <c r="C4" s="4">
-        <f>8631360/150</f>
-        <v>57542.400000000001</v>
+        <f>(8631360+25408156)/150</f>
+        <v>226930.10666666666</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1979,7 +1980,8 @@
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <v>1064984</v>
+        <f>1064984*1.05</f>
+        <v>1118233.2</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
updated pricing to day ahead LMP
</commit_message>
<xml_diff>
--- a/projects/virginia/capacity_sweep/scenarios.xlsx
+++ b/projects/virginia/capacity_sweep/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71A7A4A8-DB5D-4321-958B-F3A255020FED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8567718F-AEFF-4A98-AB0F-4201E4BC0E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_only" sheetId="11" r:id="rId1"/>
@@ -796,7 +796,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
@@ -1494,7 +1494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572AD386-7007-4195-B318-4BA3867819FF}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -1842,7 +1842,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C212AEE-474A-42BF-8E8E-5CD7BCCCC67E}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated analysis and post processing
</commit_message>
<xml_diff>
--- a/projects/virginia/capacity_sweep/scenarios.xlsx
+++ b/projects/virginia/capacity_sweep/scenarios.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8567718F-AEFF-4A98-AB0F-4201E4BC0E77}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D9ED87-F89D-43BC-93C5-1278C2AF0680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="wind_only" sheetId="11" r:id="rId1"/>
@@ -451,7 +451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBE905B-6C91-4020-936E-5C369A819AB5}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -797,7 +797,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -933,8 +933,8 @@
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <f>2248*1000</f>
-        <v>2248000</v>
+        <f>2569*1000</f>
+        <v>2569000</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1146,7 +1146,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1282,8 +1282,8 @@
         <v>26</v>
       </c>
       <c r="C6" s="4">
-        <f>5038*1000</f>
-        <v>5038000</v>
+        <f>5756*1000</f>
+        <v>5756000</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1842,8 +1842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C212AEE-474A-42BF-8E8E-5CD7BCCCC67E}">
   <dimension ref="A1:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
updated analysis to take results from sizing and cost studies as inputs
</commit_message>
<xml_diff>
--- a/projects/virginia/capacity_sweep/scenarios.xlsx
+++ b/projects/virginia/capacity_sweep/scenarios.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D9ED87-F89D-43BC-93C5-1278C2AF0680}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0B4D9D-BC8C-4F81-8439-18A0A7A0368F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,10 @@
     <sheet name="4_hr_batt" sheetId="9" r:id="rId2"/>
     <sheet name="10_hr_batt" sheetId="12" r:id="rId3"/>
     <sheet name="10_hr_ocaes" sheetId="10" r:id="rId4"/>
-    <sheet name="24_hr_ocaes" sheetId="13" r:id="rId5"/>
+    <sheet name="24_hr_ocaes" sheetId="14" r:id="rId5"/>
+    <sheet name="48_hr_ocaes" sheetId="15" r:id="rId6"/>
+    <sheet name="72_hr_ocaes" sheetId="16" r:id="rId7"/>
+    <sheet name="168_hr_ocaes" sheetId="17" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="23">
   <si>
     <t>Ref.</t>
   </si>
@@ -77,25 +80,10 @@
     <t>eta_storage</t>
   </si>
   <si>
-    <t>C_well</t>
-  </si>
-  <si>
-    <t>C_cmp</t>
-  </si>
-  <si>
     <t>C_exp</t>
   </si>
   <si>
-    <t>V_cmp</t>
-  </si>
-  <si>
     <t>V_exp</t>
-  </si>
-  <si>
-    <t>F_well</t>
-  </si>
-  <si>
-    <t>F_cmp</t>
   </si>
   <si>
     <t>F_exp</t>
@@ -113,14 +101,17 @@
     <t>[$/MW]</t>
   </si>
   <si>
-    <t>uniform</t>
+    <t>script overwrites</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,6 +121,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -160,17 +158,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="43" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -449,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBE905B-6C91-4020-936E-5C369A819AB5}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A5" sqref="A5:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,7 +538,7 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -558,12 +558,12 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
         <v>0</v>
       </c>
       <c r="D5" t="s">
@@ -581,10 +581,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>25</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C8" s="2">
         <v>0</v>
@@ -650,10 +650,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -668,121 +668,6 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="2">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="2">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
         <v>0</v>
       </c>
     </row>
@@ -794,16 +679,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -840,7 +725,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>4</v>
       </c>
       <c r="D2" t="s">
@@ -863,7 +748,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.86</v>
       </c>
       <c r="D3" t="s">
@@ -884,10 +769,11 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <f>2248*1000</f>
+        <v>2248000</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -904,13 +790,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="4">
+        <f>10*1000</f>
+        <v>10000</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -927,14 +814,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <f>2569*1000</f>
-        <v>2569000</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <f>0.03/100*1000</f>
+        <v>0.3</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -951,13 +838,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="C7" s="3">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -974,14 +861,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4">
-        <f>0.03/100*1000</f>
-        <v>0.3</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -998,13 +884,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1016,122 +902,6 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4">
-        <f>10*1000</f>
-        <v>10000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
         <v>0</v>
       </c>
     </row>
@@ -1143,16 +913,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E6042A-59F1-47A5-BAF9-EFE99B5A724F}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1189,7 +959,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -1212,7 +982,7 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>0.86</v>
       </c>
       <c r="D3" t="s">
@@ -1233,10 +1003,11 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="4">
+        <f>5038*1000</f>
+        <v>5038000</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1253,13 +1024,14 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="4">
+        <f>10*1000</f>
+        <v>10000</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1276,14 +1048,14 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <f>5756*1000</f>
-        <v>5756000</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <f>0.03/100*1000</f>
+        <v>0.3</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1300,13 +1072,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
+      <c r="C7" s="3">
+        <v>10</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1323,14 +1095,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="4">
-        <f>0.03/100*1000</f>
-        <v>0.3</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>10</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1347,13 +1118,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1365,122 +1136,6 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="4">
-        <f>10*1000</f>
-        <v>10000</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4">
-        <v>10</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
-        <v>10</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
         <v>0</v>
       </c>
     </row>
@@ -1492,10 +1147,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572AD386-7007-4195-B318-4BA3867819FF}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1503,6 +1158,7 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1538,7 +1194,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>10</v>
       </c>
       <c r="D2" t="s">
@@ -1561,20 +1217,23 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.79</v>
+      <c r="C3" s="2">
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>0.77500000000000002</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.79300000000000004</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1582,11 +1241,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4">
-        <f>(8631360+25408156)/150</f>
-        <v>226930.10666666666</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1599,17 +1257,20 @@
       </c>
       <c r="G4">
         <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>16300</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1626,14 +1287,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <f>1064984*1.05</f>
-        <v>1118233.2</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.24</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1650,13 +1310,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="3">
         <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1673,13 +1333,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
         <v>25</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4.62</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -1696,13 +1356,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -1714,121 +1374,6 @@
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4">
-        <v>25</v>
-      </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4">
-        <v>25</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
-        <v>25</v>
-      </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
         <v>0</v>
       </c>
     </row>
@@ -1839,11 +1384,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C212AEE-474A-42BF-8E8E-5CD7BCCCC67E}">
-  <dimension ref="A1:H14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B574E9F1-E5FD-4CBF-A0EC-91AD91E066EC}">
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1851,6 +1396,7 @@
     <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -1886,7 +1432,7 @@
       <c r="B2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>24</v>
       </c>
       <c r="D2" t="s">
@@ -1909,20 +1455,23 @@
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="4">
-        <v>0.79</v>
+      <c r="C3" s="2">
+        <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>0.77500000000000002</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>0.79300000000000004</v>
+        <v>0</v>
       </c>
       <c r="G3">
         <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -1930,11 +1479,10 @@
         <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="4">
-        <f>(8631360+25408156)/150</f>
-        <v>226930.10666666666</v>
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1947,17 +1495,20 @@
       </c>
       <c r="G4">
         <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>16300</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1974,14 +1525,13 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="4">
-        <f>1064984*1.05</f>
-        <v>1118233.2</v>
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.24</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1998,13 +1548,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" s="3">
         <v>25</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2021,13 +1571,13 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
         <v>25</v>
-      </c>
-      <c r="C8" s="4">
-        <v>4.62</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -2044,13 +1594,251 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88485715-ABCE-41DA-B731-B26B8EA84D7A}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>16300</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
         <v>20</v>
       </c>
+      <c r="C6" s="3">
+        <v>9.24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
       <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="2">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
@@ -2065,118 +1853,479 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DFF53B-FB7A-4677-A63D-19B0C8D86B5F}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>72</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="2">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="2">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>16300</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="4">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
         <v>25</v>
       </c>
-      <c r="D12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
         <v>25</v>
       </c>
-      <c r="D14" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A92BC3-E457-4A1B-B86A-8D54AF7C99D1}">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3">
+        <v>168</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3">
+        <v>16300</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="3">
+        <v>9.24</v>
+      </c>
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>25</v>
+      </c>
+      <c r="D7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>25</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added capacity credits to revenue stream
</commit_message>
<xml_diff>
--- a/projects/virginia/capacity_sweep/scenarios.xlsx
+++ b/projects/virginia/capacity_sweep/scenarios.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0B4D9D-BC8C-4F81-8439-18A0A7A0368F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A5797-05B8-439D-A196-D2827C50E5BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,18 +22,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="24">
   <si>
     <t>Ref.</t>
   </si>
@@ -102,6 +96,9 @@
   </si>
   <si>
     <t>script overwrites</t>
+  </si>
+  <si>
+    <t>CC_exp</t>
   </si>
 </sst>
 </file>
@@ -449,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCBE905B-6C91-4020-936E-5C369A819AB5}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:G5"/>
+      <selection activeCell="G4" sqref="A4:G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -535,10 +532,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C4" s="2">
         <v>0</v>
@@ -558,10 +555,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C5" s="2">
         <v>0</v>
@@ -581,10 +578,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -604,10 +601,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="2">
         <v>0</v>
@@ -627,7 +624,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -650,7 +647,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -668,6 +665,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -679,10 +699,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,86 +786,86 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <f>2248*1000</f>
         <v>2248000</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <f>10*1000</f>
         <v>10000</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="3">
         <f>0.03/100*1000</f>
         <v>0.3</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3">
-        <v>10</v>
-      </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -861,7 +881,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -884,7 +904,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -902,6 +922,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -913,10 +956,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4E6042A-59F1-47A5-BAF9-EFE99B5A724F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1000,86 +1043,86 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C5" s="4">
         <f>5038*1000</f>
         <v>5038000</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C6" s="4">
         <f>10*1000</f>
         <v>10000</v>
       </c>
-      <c r="D5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="D6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>16</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C7" s="3">
         <f>0.03/100*1000</f>
         <v>0.3</v>
       </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="3">
-        <v>10</v>
-      </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
@@ -1095,7 +1138,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1118,7 +1161,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1136,6 +1179,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -1147,10 +1213,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{572AD386-7007-4195-B318-4BA3867819FF}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1238,13 +1304,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1257,20 +1323,17 @@
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>16300</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1283,17 +1346,20 @@
       </c>
       <c r="G5">
         <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>9.24</v>
+        <v>16300</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1310,13 +1376,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>9.24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1333,7 +1399,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1356,7 +1422,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1374,6 +1440,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -1385,10 +1474,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B574E9F1-E5FD-4CBF-A0EC-91AD91E066EC}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1476,13 +1565,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1495,20 +1584,17 @@
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>16300</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1521,17 +1607,20 @@
       </c>
       <c r="G5">
         <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>9.24</v>
+        <v>16300</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1548,13 +1637,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>9.24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1571,7 +1660,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1594,7 +1683,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1612,6 +1701,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -1623,10 +1735,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88485715-ABCE-41DA-B731-B26B8EA84D7A}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1714,13 +1826,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1733,20 +1845,17 @@
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>16300</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1759,17 +1868,20 @@
       </c>
       <c r="G5">
         <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>9.24</v>
+        <v>16300</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -1786,13 +1898,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>9.24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -1809,7 +1921,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -1832,7 +1944,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -1850,6 +1962,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -1861,10 +1996,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9DFF53B-FB7A-4677-A63D-19B0C8D86B5F}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1952,13 +2087,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -1971,20 +2106,17 @@
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>16300</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -1997,17 +2129,20 @@
       </c>
       <c r="G5">
         <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>9.24</v>
+        <v>16300</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -2024,13 +2159,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>9.24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2047,7 +2182,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2070,7 +2205,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -2088,6 +2223,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>
@@ -2099,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29A92BC3-E457-4A1B-B86A-8D54AF7C99D1}">
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2190,13 +2348,13 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1</v>
       </c>
       <c r="D4" t="s">
         <v>9</v>
@@ -2209,20 +2367,17 @@
       </c>
       <c r="G4">
         <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="3">
-        <v>16300</v>
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>9</v>
@@ -2235,17 +2390,20 @@
       </c>
       <c r="G5">
         <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3">
-        <v>9.24</v>
+        <v>16300</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
@@ -2262,13 +2420,13 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3">
-        <v>25</v>
+        <v>9.24</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -2285,7 +2443,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
@@ -2308,7 +2466,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -2326,6 +2484,29 @@
         <v>0</v>
       </c>
       <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>25</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
         <v>0</v>
       </c>
     </row>

</xml_diff>